<commit_message>
feat: Update README for clarity and localization; modify budget reader settings for consistency
</commit_message>
<xml_diff>
--- a/data/sample_padrao1 - Copia.xlsx
+++ b/data/sample_padrao1 - Copia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="11_2B5A8FE7125C5C426140C57430267256DF8CDB53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F6AAE74-3B1A-4EC4-90BE-B7691BD74914}"/>
+  <xr:revisionPtr revIDLastSave="251" documentId="11_2B5A8FE7125C5C426140C57430267256DF8CDB53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7B8F9A8-EBD7-446B-B053-B2E3C4FE700D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="73">
   <si>
     <t>ITAÚ UNIBANCO S/A - Ag. 4830 - SANTOS - BOQUEIRÃO - SP</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Vidros</t>
+  </si>
+  <si>
+    <t>Quant</t>
   </si>
 </sst>
 </file>
@@ -366,30 +369,12 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -406,6 +391,24 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -424,10 +427,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -717,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -728,376 +727,376 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" s="16" customFormat="1" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="19" t="s">
+      <c r="F5" s="23"/>
+      <c r="G5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="17"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="22">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="16">
         <v>69368.350000000006</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="14">
         <v>100</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15">
         <f>SUM(G11:G20)</f>
         <v>7402.7100000000009</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="15">
         <f>SUM(H11:H20)</f>
         <v>10.68</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="17">
         <v>10.9</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="17">
         <v>11.97</v>
       </c>
-      <c r="F11" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G11" s="23">
+      <c r="F11" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G11" s="17">
         <v>169.64</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="17">
         <v>0.24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="17">
         <v>5</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="17">
         <v>99.94</v>
       </c>
-      <c r="F12" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G12" s="23">
+      <c r="F12" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G12" s="17">
         <v>649.62</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="17">
         <v>0.94</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="17">
         <v>36.590000000000003</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="17">
         <v>20.89</v>
       </c>
-      <c r="F13" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G13" s="23">
+      <c r="F13" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G13" s="17">
         <v>993.8</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="17">
         <v>1.43</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="17">
         <v>4.3600000000000003</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="17">
         <v>15.95</v>
       </c>
-      <c r="F14" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G14" s="23">
+      <c r="F14" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G14" s="17">
         <v>90.41</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="17">
         <v>0.13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="17">
         <v>7.38</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="17">
         <v>24.98</v>
       </c>
-      <c r="F15" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G15" s="23">
+      <c r="F15" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G15" s="17">
         <v>239.69</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="17">
         <v>0.35</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="17">
         <v>5</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="17">
         <v>320.83999999999997</v>
       </c>
-      <c r="F16" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G16" s="25">
+      <c r="F16" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G16" s="19">
         <v>2085.4299999999998</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="17">
         <v>3.01</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="17">
         <v>4.75</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="17">
         <v>12.01</v>
       </c>
-      <c r="F17" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G17" s="23">
+      <c r="F17" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G17" s="17">
         <v>74.180000000000007</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="17">
         <v>0.11</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="17">
         <v>11</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="17">
         <v>10.93</v>
       </c>
-      <c r="F18" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G18" s="23">
+      <c r="F18" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G18" s="17">
         <v>156.31</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="17">
         <v>0.23</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="17">
         <v>9</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="17">
         <v>83.76</v>
       </c>
-      <c r="F19" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G19" s="23">
+      <c r="F19" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G19" s="17">
         <v>979.96</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="17">
         <v>1.41</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="17">
         <v>26.61</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="17">
         <v>56.76</v>
       </c>
-      <c r="F20" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G20" s="25">
+      <c r="F20" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G20" s="19">
         <v>1963.67</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H20" s="17">
         <v>2.83</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="20">
         <f>SUM(G22:G23)</f>
         <v>22074.27</v>
       </c>
@@ -1107,61 +1106,61 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24" t="s">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="17">
         <v>13.58</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="17">
         <v>289.02999999999997</v>
       </c>
-      <c r="F22" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G22" s="25">
+      <c r="F22" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G22" s="19">
         <v>5102.54</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="17">
         <v>7.36</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="17">
         <v>26.61</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="17">
         <v>490.61</v>
       </c>
-      <c r="F23" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G23" s="25">
+      <c r="F23" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G23" s="19">
         <v>16971.73</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="17">
         <v>24.47</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="20">
         <f>SUM(G25:G26)</f>
         <v>7523.33</v>
       </c>
@@ -1171,50 +1170,50 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="17">
         <v>2.94</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="17">
         <v>916.37</v>
       </c>
-      <c r="F25" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G25" s="25">
+      <c r="F25" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G25" s="19">
         <v>3502.35</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="17">
         <v>5.05</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="17">
         <v>4.4400000000000004</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="17">
         <v>696.64</v>
       </c>
-      <c r="F26" s="23">
-        <v>1.3</v>
-      </c>
-      <c r="G26" s="25">
+      <c r="F26" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="G26" s="19">
         <v>4020.98</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="17">
         <v>5.8</v>
       </c>
     </row>
@@ -1238,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,17 +1255,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -1280,56 +1279,56 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>

</xml_diff>